<commit_message>
Update Excel sheet with correct test case order
</commit_message>
<xml_diff>
--- a/IT23674394.xlsx
+++ b/IT23674394.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\playwright assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\IT23674394\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C936D123-41DF-4BC5-8812-5203B9B75501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F04B3F-7A2D-493E-A8B3-7A76DF233282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,9 +526,6 @@
     <t>Question mark retained at end.</t>
   </si>
   <si>
-    <t>Correct word choice for "gaththada".</t>
-  </si>
-  <si>
     <t>Imperative/Command form recognized.</t>
   </si>
   <si>
@@ -1037,6 +1034,9 @@
   </si>
   <si>
     <t>ඔයාට කොහොමද?</t>
+  </si>
+  <si>
+    <t>Correct word choice for "kohomadha".</t>
   </si>
 </sst>
 </file>
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E10:E11"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1458,49 +1458,49 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>335</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>336</v>
       </c>
       <c r="F2" t="s">
-        <v>117</v>
+        <v>336</v>
       </c>
       <c r="G2" t="s">
         <v>154</v>
       </c>
       <c r="H2" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="I2" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H3" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I3" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
-        <v>158</v>
+        <v>337</v>
       </c>
       <c r="I4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1529,7 +1529,7 @@
         <v>159</v>
       </c>
       <c r="I6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1537,7 +1537,7 @@
         <v>160</v>
       </c>
       <c r="I7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1545,12 +1545,12 @@
         <v>161</v>
       </c>
       <c r="I8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1579,7 +1579,7 @@
         <v>162</v>
       </c>
       <c r="I10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1587,7 +1587,7 @@
         <v>163</v>
       </c>
       <c r="I11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1595,12 +1595,12 @@
         <v>164</v>
       </c>
       <c r="I12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1608,49 +1608,49 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
         <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>336</v>
+        <v>83</v>
       </c>
       <c r="E14" t="s">
-        <v>337</v>
+        <v>117</v>
       </c>
       <c r="F14" t="s">
-        <v>337</v>
+        <v>117</v>
       </c>
       <c r="G14" t="s">
         <v>154</v>
       </c>
       <c r="H14" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="I14" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H15" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="I15" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H16" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="I16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1676,31 +1676,31 @@
         <v>154</v>
       </c>
       <c r="H18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1726,31 +1726,31 @@
         <v>154</v>
       </c>
       <c r="H22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I24" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1776,31 +1776,31 @@
         <v>154</v>
       </c>
       <c r="H26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1826,31 +1826,31 @@
         <v>154</v>
       </c>
       <c r="H30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1876,31 +1876,31 @@
         <v>154</v>
       </c>
       <c r="H34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I35" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I36" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I37" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1926,31 +1926,31 @@
         <v>154</v>
       </c>
       <c r="H38" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I39" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I41" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -1976,31 +1976,31 @@
         <v>154</v>
       </c>
       <c r="H42" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I42" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H43" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H44" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I44" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -2026,31 +2026,31 @@
         <v>154</v>
       </c>
       <c r="H46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I46" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H47" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I47" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H48" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I48" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -2076,31 +2076,31 @@
         <v>154</v>
       </c>
       <c r="H50" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I50" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I51" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H52" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I52" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I53" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -2126,31 +2126,31 @@
         <v>154</v>
       </c>
       <c r="H54" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I54" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I55" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I56" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I57" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -2176,31 +2176,31 @@
         <v>154</v>
       </c>
       <c r="H58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I58" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H59" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I59" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H60" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I60" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I61" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -2226,31 +2226,31 @@
         <v>154</v>
       </c>
       <c r="H62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H63" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I63" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I65" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -2276,31 +2276,31 @@
         <v>154</v>
       </c>
       <c r="H66" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I66" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H67" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I67" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H68" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I68" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
@@ -2326,31 +2326,31 @@
         <v>154</v>
       </c>
       <c r="H70" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I70" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H72" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I72" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I73" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -2376,31 +2376,31 @@
         <v>154</v>
       </c>
       <c r="H74" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I74" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I75" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I76" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I77" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -2426,31 +2426,31 @@
         <v>154</v>
       </c>
       <c r="H78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I78" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I79" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H80" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I80" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I81" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -2476,31 +2476,31 @@
         <v>154</v>
       </c>
       <c r="H82" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I82" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H83" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I83" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H84" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I84" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I85" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
@@ -2526,31 +2526,31 @@
         <v>154</v>
       </c>
       <c r="H86" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I86" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I87" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H88" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I88" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I89" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
@@ -2576,31 +2576,31 @@
         <v>154</v>
       </c>
       <c r="H90" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I90" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H91" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I91" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H92" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I92" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I93" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
@@ -2626,31 +2626,31 @@
         <v>154</v>
       </c>
       <c r="H94" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I94" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H95" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I95" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H96" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I96" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I97" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
@@ -2676,31 +2676,31 @@
         <v>155</v>
       </c>
       <c r="H98" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I98" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H99" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I99" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H100" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I100" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I101" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
@@ -2726,31 +2726,31 @@
         <v>155</v>
       </c>
       <c r="H102" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I102" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H103" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I103" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H104" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I104" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I105" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
@@ -2776,31 +2776,31 @@
         <v>155</v>
       </c>
       <c r="H106" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I106" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H107" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I107" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H108" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I108" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I109" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
@@ -2826,31 +2826,31 @@
         <v>155</v>
       </c>
       <c r="H110" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I110" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H111" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I111" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H112" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I112" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I113" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
@@ -2876,31 +2876,31 @@
         <v>155</v>
       </c>
       <c r="H114" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I114" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H115" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I115" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H116" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I116" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I117" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
@@ -2926,31 +2926,31 @@
         <v>155</v>
       </c>
       <c r="H118" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I118" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H119" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I119" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H120" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I120" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I121" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
@@ -2976,31 +2976,31 @@
         <v>155</v>
       </c>
       <c r="H122" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I122" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H123" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I123" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H124" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I124" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I125" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
@@ -3026,31 +3026,31 @@
         <v>155</v>
       </c>
       <c r="H126" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I126" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H127" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I127" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H128" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I128" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I129" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
@@ -3076,31 +3076,31 @@
         <v>155</v>
       </c>
       <c r="H130" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I130" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H131" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I131" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H132" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I132" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I133" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
@@ -3126,31 +3126,31 @@
         <v>155</v>
       </c>
       <c r="H134" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I134" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H135" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I135" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H136" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I136" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I137" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
@@ -3176,23 +3176,23 @@
         <v>154</v>
       </c>
       <c r="H138" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I138" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H139" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I139" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H140" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I140" t="s">
         <v>82</v>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I141" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final updates: Complete test cases and automation
</commit_message>
<xml_diff>
--- a/IT23674394.xlsx
+++ b/IT23674394.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\IT23674394\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\playwright assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F04B3F-7A2D-493E-A8B3-7A76DF233282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E6CA30-C16E-4CF2-A689-0F71351B9B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1030,13 +1030,13 @@
     <t>Functional UI</t>
   </si>
   <si>
-    <t>oyaata kohomadha?</t>
-  </si>
-  <si>
-    <t>ඔයාට කොහොමද?</t>
-  </si>
-  <si>
     <t>Correct word choice for "kohomadha".</t>
+  </si>
+  <si>
+    <t>oyaa sathutindha inne?</t>
+  </si>
+  <si>
+    <t>ඔයා සතුටින්ද ඉන්නේ?</t>
   </si>
 </sst>
 </file>
@@ -1407,7 +1407,7 @@
   <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1464,13 +1464,13 @@
         <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G2" t="s">
         <v>154</v>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="I4" t="s">
         <v>262</v>

</xml_diff>